<commit_message>
added first results of user study, changed border colors of devices to device colors, started implementing object observing
</commit_message>
<xml_diff>
--- a/User Study/participants.xlsx
+++ b/User Study/participants.xlsx
@@ -24,23 +24,43 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>Hantao</t>
   </si>
   <si>
-    <t>Marica Bertarini</t>
+    <t>Amir Tafreshi</t>
   </si>
   <si>
-    <t>Amir Tafreshi</t>
+    <t>Matthias</t>
+  </si>
+  <si>
+    <t>Steven</t>
+  </si>
+  <si>
+    <t>Nicola</t>
+  </si>
+  <si>
+    <t>Number of participants</t>
+  </si>
+  <si>
+    <t>Sybil</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -68,10 +88,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -352,180 +373,192 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B60"/>
+  <dimension ref="A1:E72"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B39" sqref="B39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1">
-        <v>42599</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+        <v>42233</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>0.33333333333333331</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>0.41666666666666669</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>0.5</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>0.58333333333333304</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D5" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E5" s="3">
+        <f>COUNTA(B1:B60)</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>0.66666666666666596</v>
       </c>
-      <c r="B6" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="E6" s="3"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
-        <v>42600</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+        <v>42234</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>0.33333333333333331</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>0.41666666666666669</v>
       </c>
       <c r="B9" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>0.5</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>0.58333333333333337</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>0.66666666666666663</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
-        <v>42601</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+        <v>42235</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <v>0.33333333333333331</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
         <v>0.41666666666666669</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
         <v>0.5</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
         <v>0.58333333333333337</v>
       </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
         <v>0.66666666666666663</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
-        <v>42602</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+        <v>42236</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
         <v>0.33333333333333331</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
         <v>0.41666666666666669</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="2">
         <v>0.5</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="2">
         <v>0.58333333333333337</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="2">
         <v>0.66666666666666663</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
-        <v>42603</v>
-      </c>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+        <v>42237</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" s="2">
         <v>0.33333333333333331</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" s="2">
         <v>0.41666666666666669</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" s="2">
         <v>0.5</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" s="2">
         <v>0.58333333333333337</v>
       </c>
-    </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B29" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" s="2">
         <v>0.66666666666666663</v>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
-        <v>42606</v>
-      </c>
-    </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+        <v>42240</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" s="2">
         <v>0.33333333333333331</v>
       </c>
@@ -547,6 +580,9 @@
       <c r="A35" s="2">
         <v>0.58333333333333337</v>
       </c>
+      <c r="B35" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" s="2">
@@ -555,7 +591,7 @@
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
-        <v>42607</v>
+        <v>42241</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
@@ -577,6 +613,9 @@
       <c r="A41" s="2">
         <v>0.58333333333333337</v>
       </c>
+      <c r="B41" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" s="2">
@@ -585,95 +624,156 @@
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
-        <v>42608</v>
+        <v>42242</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" s="2">
-        <v>0.33333333333333331</v>
+        <v>0.375</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" s="2">
-        <v>0.41666666666666669</v>
+        <v>0.45833333333333331</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" s="2">
-        <v>0.5</v>
+        <v>0.54166666666666663</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" s="2">
-        <v>0.58333333333333337</v>
+        <v>0.625</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A48" s="2">
-        <v>0.66666666666666663</v>
+      <c r="A48" s="1">
+        <v>42243</v>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A49" s="1">
-        <v>42609</v>
+      <c r="A49" s="2">
+        <v>0.375</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A50" s="2">
-        <v>0.33333333333333331</v>
+        <v>0.45833333333333331</v>
       </c>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A51" s="2">
-        <v>0.41666666666666669</v>
+        <v>0.54166666666666663</v>
       </c>
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A52" s="2">
-        <v>0.5</v>
+        <v>0.625</v>
       </c>
     </row>
     <row r="53" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A53" s="2">
-        <v>0.58333333333333337</v>
+      <c r="A53" s="1">
+        <v>42244</v>
       </c>
     </row>
     <row r="54" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A54" s="2">
-        <v>0.66666666666666663</v>
+        <v>0.375</v>
       </c>
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A55" s="1">
-        <v>42610</v>
+      <c r="A55" s="2">
+        <v>0.45833333333333331</v>
       </c>
     </row>
     <row r="56" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A56" s="2">
-        <v>0.33333333333333331</v>
+        <v>0.54166666666666663</v>
       </c>
     </row>
     <row r="57" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A57" s="2">
-        <v>0.41666666666666669</v>
+        <v>0.625</v>
       </c>
     </row>
     <row r="58" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A58" s="2">
-        <v>0.5</v>
+      <c r="A58" s="1">
+        <v>42247</v>
       </c>
     </row>
     <row r="59" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A59" s="2">
-        <v>0.58333333333333337</v>
+        <v>0.375</v>
       </c>
     </row>
     <row r="60" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A60" s="2">
-        <v>0.66666666666666663</v>
+        <v>0.45833333333333331</v>
+      </c>
+    </row>
+    <row r="61" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A61" s="2">
+        <v>0.54166666666666663</v>
+      </c>
+    </row>
+    <row r="62" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A62" s="2">
+        <v>0.625</v>
+      </c>
+    </row>
+    <row r="63" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A63" s="1">
+        <v>42248</v>
+      </c>
+    </row>
+    <row r="64" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A64" s="2">
+        <v>0.375</v>
+      </c>
+    </row>
+    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A65" s="2">
+        <v>0.45833333333333331</v>
+      </c>
+    </row>
+    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A66" s="2">
+        <v>0.54166666666666663</v>
+      </c>
+    </row>
+    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A67" s="2">
+        <v>0.625</v>
+      </c>
+    </row>
+    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A68" s="1">
+        <v>42249</v>
+      </c>
+    </row>
+    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A69" s="2">
+        <v>0.375</v>
+      </c>
+    </row>
+    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A70" s="2">
+        <v>0.45833333333333331</v>
+      </c>
+    </row>
+    <row r="71" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A71" s="2">
+        <v>0.54166666666666663</v>
+      </c>
+    </row>
+    <row r="72" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A72" s="2">
+        <v>0.625</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
updated study results, improved layout of tool, improved function debugging to show device on which function is called
</commit_message>
<xml_diff>
--- a/User Study/participants.xlsx
+++ b/User Study/participants.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>Hantao</t>
   </si>
@@ -45,6 +45,9 @@
   </si>
   <si>
     <t>Sybil</t>
+  </si>
+  <si>
+    <t>Jakub</t>
   </si>
 </sst>
 </file>
@@ -373,10 +376,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E72"/>
+  <dimension ref="A1:E71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B39" sqref="B39"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="B60" sqref="B60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -415,7 +418,7 @@
       </c>
       <c r="E5" s="3">
         <f>COUNTA(B1:B60)</f>
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -652,123 +655,121 @@
         <v>42243</v>
       </c>
     </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" s="2">
         <v>0.375</v>
       </c>
     </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" s="2">
         <v>0.45833333333333331</v>
       </c>
     </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" s="2">
         <v>0.54166666666666663</v>
       </c>
     </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" s="2">
         <v>0.625</v>
       </c>
     </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" s="1">
         <v>42244</v>
       </c>
     </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" s="2">
         <v>0.375</v>
       </c>
     </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" s="2">
         <v>0.45833333333333331</v>
       </c>
     </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56" s="2">
         <v>0.54166666666666663</v>
       </c>
     </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57" s="2">
         <v>0.625</v>
       </c>
     </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58" s="1">
         <v>42247</v>
       </c>
     </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59" s="2">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="B59" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A60" s="2">
+        <v>0.54166666666666663</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A61" s="2">
+        <v>0.625</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A62" s="1">
+        <v>42248</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A63" s="2">
         <v>0.375</v>
       </c>
     </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A60" s="2">
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A64" s="2">
         <v>0.45833333333333331</v>
-      </c>
-    </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A61" s="2">
-        <v>0.54166666666666663</v>
-      </c>
-    </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A62" s="2">
-        <v>0.625</v>
-      </c>
-    </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A63" s="1">
-        <v>42248</v>
-      </c>
-    </row>
-    <row r="64" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A64" s="2">
-        <v>0.375</v>
       </c>
     </row>
     <row r="65" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A65" s="2">
-        <v>0.45833333333333331</v>
+        <v>0.54166666666666663</v>
       </c>
     </row>
     <row r="66" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A66" s="2">
-        <v>0.54166666666666663</v>
+        <v>0.625</v>
       </c>
     </row>
     <row r="67" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A67" s="2">
-        <v>0.625</v>
+      <c r="A67" s="1">
+        <v>42249</v>
       </c>
     </row>
     <row r="68" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A68" s="1">
-        <v>42249</v>
+      <c r="A68" s="2">
+        <v>0.375</v>
       </c>
     </row>
     <row r="69" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A69" s="2">
-        <v>0.375</v>
+        <v>0.45833333333333331</v>
       </c>
     </row>
     <row r="70" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A70" s="2">
-        <v>0.45833333333333331</v>
+        <v>0.54166666666666663</v>
       </c>
     </row>
     <row r="71" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A71" s="2">
-        <v>0.54166666666666663</v>
-      </c>
-    </row>
-    <row r="72" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A72" s="2">
         <v>0.625</v>
       </c>
     </row>

</xml_diff>